<commit_message>
Excel files upload to Etsy - refactoring to use jobs and upload photos
</commit_message>
<xml_diff>
--- a/zencommerce/static/ListingsTest.xlsx
+++ b/zencommerce/static/ListingsTest.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vserh/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4EA73B7-D9B2-C84B-89FF-292BA1A022F6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{995A6CBA-9DAD-1D48-AEFD-681E9B1429E4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="420" yWindow="800" windowWidth="29740" windowHeight="18300" xr2:uid="{DED3D6E4-F41E-9C45-87F1-9A249DE231F9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="29">
   <si>
     <t>Title</t>
   </si>
@@ -36,18 +36,6 @@
     <t>Price</t>
   </si>
   <si>
-    <t>Bla bla bla 1</t>
-  </si>
-  <si>
-    <t>Test 2</t>
-  </si>
-  <si>
-    <t>Test 3</t>
-  </si>
-  <si>
-    <t>Test 4</t>
-  </si>
-  <si>
     <t>Quantity</t>
   </si>
   <si>
@@ -87,15 +75,6 @@
     <t>Currency code</t>
   </si>
   <si>
-    <t>Bla bla bla 2</t>
-  </si>
-  <si>
-    <t>Bla bla bla 3</t>
-  </si>
-  <si>
-    <t>Bla bla bla 4</t>
-  </si>
-  <si>
     <t>Is digital</t>
   </si>
   <si>
@@ -111,19 +90,28 @@
     <t>Listing id</t>
   </si>
   <si>
-    <t>Test 5 - Updated</t>
-  </si>
-  <si>
-    <t>Bla bla bla 5 - Updated</t>
-  </si>
-  <si>
-    <t>tag3,tag4,tag555</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
-    <t>Test 1 - Updated</t>
+    <t>Pretty handmade T-Shirt</t>
+  </si>
+  <si>
+    <t>Handmade T-Shirt - white</t>
+  </si>
+  <si>
+    <t>Handmade high grade item. And so on, and so on…</t>
+  </si>
+  <si>
+    <t>Handmade T-Shirt - blue</t>
+  </si>
+  <si>
+    <t>Handmade T-Shirt - black</t>
+  </si>
+  <si>
+    <t>Handmade T-Shirt - green</t>
+  </si>
+  <si>
+    <t>tag3,tag4,tag5</t>
   </si>
 </sst>
 </file>
@@ -496,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{089C0892-B9BA-EA45-8112-D49AFC0FB42F}">
   <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -518,13 +506,13 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -536,31 +524,31 @@
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -568,19 +556,19 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E2" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="F2">
         <v>0.2</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -589,22 +577,22 @@
         <v>449</v>
       </c>
       <c r="J2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="K2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="M2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="N2">
         <v>87520071257</v>
       </c>
       <c r="O2" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
@@ -612,19 +600,19 @@
         <v>2</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F3">
         <v>0.25</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="H3">
         <v>2</v>
@@ -633,22 +621,22 @@
         <v>449</v>
       </c>
       <c r="J3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="K3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="M3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="N3">
         <v>87520071257</v>
       </c>
       <c r="O3" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -656,19 +644,19 @@
         <v>3</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F4" s="2">
         <v>0.3</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="H4">
         <v>3</v>
@@ -677,22 +665,22 @@
         <v>449</v>
       </c>
       <c r="J4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="K4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="M4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="N4">
         <v>87520071257</v>
       </c>
       <c r="O4" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -700,19 +688,19 @@
         <v>4</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F5" s="2">
         <v>0.4</v>
       </c>
       <c r="G5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="H5">
         <v>4</v>
@@ -721,22 +709,22 @@
         <v>449</v>
       </c>
       <c r="J5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="K5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="M5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="N5">
         <v>87520071257</v>
       </c>
       <c r="O5" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
@@ -744,19 +732,19 @@
         <v>5</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F6" s="2">
         <v>0.6</v>
       </c>
       <c r="G6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="H6">
         <v>10</v>
@@ -765,22 +753,22 @@
         <v>449</v>
       </c>
       <c r="J6" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="K6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="M6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="N6">
         <v>87520071257</v>
       </c>
       <c r="O6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>